<commit_message>
merge sheets are not run if any overrides are there
</commit_message>
<xml_diff>
--- a/data/merge_bornpowerindex.xlsx
+++ b/data/merge_bornpowerindex.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="591">
   <si>
     <t>Index</t>
   </si>
@@ -2180,9 +2180,6 @@
       <c r="D2" t="s">
         <v>463</v>
       </c>
-      <c r="E2" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -2197,9 +2194,6 @@
       <c r="D3" t="s">
         <v>463</v>
       </c>
-      <c r="E3" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -2214,9 +2208,6 @@
       <c r="D4" t="s">
         <v>463</v>
       </c>
-      <c r="E4" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -2231,9 +2222,6 @@
       <c r="D5" t="s">
         <v>464</v>
       </c>
-      <c r="E5" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -2248,9 +2236,6 @@
       <c r="D6" t="s">
         <v>463</v>
       </c>
-      <c r="E6" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -2265,9 +2250,6 @@
       <c r="D7" t="s">
         <v>465</v>
       </c>
-      <c r="E7" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -2282,9 +2264,6 @@
       <c r="D8" t="s">
         <v>463</v>
       </c>
-      <c r="E8" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -2299,9 +2278,6 @@
       <c r="D9" t="s">
         <v>466</v>
       </c>
-      <c r="E9" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -2316,9 +2292,6 @@
       <c r="D10" t="s">
         <v>467</v>
       </c>
-      <c r="E10" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -2333,9 +2306,6 @@
       <c r="D11" t="s">
         <v>463</v>
       </c>
-      <c r="E11" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -2350,9 +2320,6 @@
       <c r="D12" t="s">
         <v>463</v>
       </c>
-      <c r="E12" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -2367,9 +2334,6 @@
       <c r="D13" t="s">
         <v>463</v>
       </c>
-      <c r="E13" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -2384,9 +2348,6 @@
       <c r="D14" t="s">
         <v>468</v>
       </c>
-      <c r="E14" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
@@ -2401,9 +2362,6 @@
       <c r="D15" t="s">
         <v>463</v>
       </c>
-      <c r="E15" t="s">
-        <v>463</v>
-      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -2418,11 +2376,8 @@
       <c r="D16" t="s">
         <v>463</v>
       </c>
-      <c r="E16" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2435,11 +2390,8 @@
       <c r="D17" t="s">
         <v>463</v>
       </c>
-      <c r="E17" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2452,11 +2404,8 @@
       <c r="D18" t="s">
         <v>463</v>
       </c>
-      <c r="E18" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2469,11 +2418,8 @@
       <c r="D19" t="s">
         <v>469</v>
       </c>
-      <c r="E19" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2486,11 +2432,8 @@
       <c r="D20" t="s">
         <v>463</v>
       </c>
-      <c r="E20" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2503,11 +2446,8 @@
       <c r="D21" t="s">
         <v>463</v>
       </c>
-      <c r="E21" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2520,11 +2460,8 @@
       <c r="D22" t="s">
         <v>470</v>
       </c>
-      <c r="E22" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2537,11 +2474,8 @@
       <c r="D23" t="s">
         <v>471</v>
       </c>
-      <c r="E23" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2554,11 +2488,8 @@
       <c r="D24" t="s">
         <v>472</v>
       </c>
-      <c r="E24" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2571,11 +2502,8 @@
       <c r="D25" t="s">
         <v>473</v>
       </c>
-      <c r="E25" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2588,11 +2516,8 @@
       <c r="D26" t="s">
         <v>463</v>
       </c>
-      <c r="E26" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2605,11 +2530,8 @@
       <c r="D27" t="s">
         <v>463</v>
       </c>
-      <c r="E27" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2622,11 +2544,8 @@
       <c r="D28" t="s">
         <v>474</v>
       </c>
-      <c r="E28" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2639,11 +2558,8 @@
       <c r="D29" t="s">
         <v>475</v>
       </c>
-      <c r="E29" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2656,11 +2572,8 @@
       <c r="D30" t="s">
         <v>463</v>
       </c>
-      <c r="E30" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2673,11 +2586,8 @@
       <c r="D31" t="s">
         <v>476</v>
       </c>
-      <c r="E31" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2690,11 +2600,8 @@
       <c r="D32" t="s">
         <v>463</v>
       </c>
-      <c r="E32" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2707,11 +2614,8 @@
       <c r="D33" t="s">
         <v>477</v>
       </c>
-      <c r="E33" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2724,11 +2628,8 @@
       <c r="D34" t="s">
         <v>478</v>
       </c>
-      <c r="E34" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2741,11 +2642,8 @@
       <c r="D35" t="s">
         <v>479</v>
       </c>
-      <c r="E35" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2758,11 +2656,8 @@
       <c r="D36" t="s">
         <v>480</v>
       </c>
-      <c r="E36" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2775,11 +2670,8 @@
       <c r="D37" t="s">
         <v>463</v>
       </c>
-      <c r="E37" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2792,11 +2684,8 @@
       <c r="D38" t="s">
         <v>463</v>
       </c>
-      <c r="E38" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2809,11 +2698,8 @@
       <c r="D39" t="s">
         <v>463</v>
       </c>
-      <c r="E39" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2826,11 +2712,8 @@
       <c r="D40" t="s">
         <v>481</v>
       </c>
-      <c r="E40" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2843,11 +2726,8 @@
       <c r="D41" t="s">
         <v>463</v>
       </c>
-      <c r="E41" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2860,11 +2740,8 @@
       <c r="D42" t="s">
         <v>463</v>
       </c>
-      <c r="E42" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2877,11 +2754,8 @@
       <c r="D43" t="s">
         <v>482</v>
       </c>
-      <c r="E43" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2894,11 +2768,8 @@
       <c r="D44" t="s">
         <v>463</v>
       </c>
-      <c r="E44" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2911,11 +2782,8 @@
       <c r="D45" t="s">
         <v>483</v>
       </c>
-      <c r="E45" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2928,11 +2796,8 @@
       <c r="D46" t="s">
         <v>463</v>
       </c>
-      <c r="E46" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2945,11 +2810,8 @@
       <c r="D47" t="s">
         <v>463</v>
       </c>
-      <c r="E47" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2962,11 +2824,8 @@
       <c r="D48" t="s">
         <v>484</v>
       </c>
-      <c r="E48" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2979,11 +2838,8 @@
       <c r="D49" t="s">
         <v>485</v>
       </c>
-      <c r="E49" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2996,11 +2852,8 @@
       <c r="D50" t="s">
         <v>463</v>
       </c>
-      <c r="E50" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3013,11 +2866,8 @@
       <c r="D51" t="s">
         <v>486</v>
       </c>
-      <c r="E51" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3030,11 +2880,8 @@
       <c r="D52" t="s">
         <v>463</v>
       </c>
-      <c r="E52" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3047,11 +2894,8 @@
       <c r="D53" t="s">
         <v>487</v>
       </c>
-      <c r="E53" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3064,11 +2908,8 @@
       <c r="D54" t="s">
         <v>488</v>
       </c>
-      <c r="E54" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3081,11 +2922,8 @@
       <c r="D55" t="s">
         <v>287</v>
       </c>
-      <c r="E55" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3098,11 +2936,8 @@
       <c r="D56" t="s">
         <v>463</v>
       </c>
-      <c r="E56" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3115,11 +2950,8 @@
       <c r="D57" t="s">
         <v>489</v>
       </c>
-      <c r="E57" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3132,11 +2964,8 @@
       <c r="D58" t="s">
         <v>490</v>
       </c>
-      <c r="E58" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3149,11 +2978,8 @@
       <c r="D59" t="s">
         <v>491</v>
       </c>
-      <c r="E59" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3166,11 +2992,8 @@
       <c r="D60" t="s">
         <v>463</v>
       </c>
-      <c r="E60" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3183,11 +3006,8 @@
       <c r="D61" t="s">
         <v>492</v>
       </c>
-      <c r="E61" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3200,11 +3020,8 @@
       <c r="D62" t="s">
         <v>493</v>
       </c>
-      <c r="E62" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3217,11 +3034,8 @@
       <c r="D63" t="s">
         <v>494</v>
       </c>
-      <c r="E63" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3234,11 +3048,8 @@
       <c r="D64" t="s">
         <v>495</v>
       </c>
-      <c r="E64" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3251,11 +3062,8 @@
       <c r="D65" t="s">
         <v>463</v>
       </c>
-      <c r="E65" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3268,11 +3076,8 @@
       <c r="D66" t="s">
         <v>496</v>
       </c>
-      <c r="E66" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3285,11 +3090,8 @@
       <c r="D67" t="s">
         <v>463</v>
       </c>
-      <c r="E67" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3302,11 +3104,8 @@
       <c r="D68" t="s">
         <v>463</v>
       </c>
-      <c r="E68" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3319,11 +3118,8 @@
       <c r="D69" t="s">
         <v>497</v>
       </c>
-      <c r="E69" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3336,11 +3132,8 @@
       <c r="D70" t="s">
         <v>302</v>
       </c>
-      <c r="E70" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3353,11 +3146,8 @@
       <c r="D71" t="s">
         <v>463</v>
       </c>
-      <c r="E71" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3370,11 +3160,8 @@
       <c r="D72" t="s">
         <v>498</v>
       </c>
-      <c r="E72" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3387,11 +3174,8 @@
       <c r="D73" t="s">
         <v>499</v>
       </c>
-      <c r="E73" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3404,11 +3188,8 @@
       <c r="D74" t="s">
         <v>500</v>
       </c>
-      <c r="E74" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3421,11 +3202,8 @@
       <c r="D75" t="s">
         <v>463</v>
       </c>
-      <c r="E75" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3438,11 +3216,8 @@
       <c r="D76" t="s">
         <v>308</v>
       </c>
-      <c r="E76" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3455,11 +3230,8 @@
       <c r="D77" t="s">
         <v>501</v>
       </c>
-      <c r="E77" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3472,11 +3244,8 @@
       <c r="D78" t="s">
         <v>463</v>
       </c>
-      <c r="E78" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3489,11 +3258,8 @@
       <c r="D79" t="s">
         <v>502</v>
       </c>
-      <c r="E79" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3506,11 +3272,8 @@
       <c r="D80" t="s">
         <v>463</v>
       </c>
-      <c r="E80" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3523,11 +3286,8 @@
       <c r="D81" t="s">
         <v>503</v>
       </c>
-      <c r="E81" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3540,11 +3300,8 @@
       <c r="D82" t="s">
         <v>504</v>
       </c>
-      <c r="E82" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3557,11 +3314,8 @@
       <c r="D83" t="s">
         <v>505</v>
       </c>
-      <c r="E83" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3574,11 +3328,8 @@
       <c r="D84" t="s">
         <v>463</v>
       </c>
-      <c r="E84" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3591,11 +3342,8 @@
       <c r="D85" t="s">
         <v>463</v>
       </c>
-      <c r="E85" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3608,11 +3356,8 @@
       <c r="D86" t="s">
         <v>463</v>
       </c>
-      <c r="E86" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3625,11 +3370,8 @@
       <c r="D87" t="s">
         <v>463</v>
       </c>
-      <c r="E87" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3642,11 +3384,8 @@
       <c r="D88" t="s">
         <v>463</v>
       </c>
-      <c r="E88" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3659,11 +3398,8 @@
       <c r="D89" t="s">
         <v>463</v>
       </c>
-      <c r="E89" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3676,11 +3412,8 @@
       <c r="D90" t="s">
         <v>463</v>
       </c>
-      <c r="E90" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3693,11 +3426,8 @@
       <c r="D91" t="s">
         <v>506</v>
       </c>
-      <c r="E91" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3710,11 +3440,8 @@
       <c r="D92" t="s">
         <v>507</v>
       </c>
-      <c r="E92" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3727,11 +3454,8 @@
       <c r="D93" t="s">
         <v>508</v>
       </c>
-      <c r="E93" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3744,11 +3468,8 @@
       <c r="D94" t="s">
         <v>509</v>
       </c>
-      <c r="E94" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3761,11 +3482,8 @@
       <c r="D95" t="s">
         <v>510</v>
       </c>
-      <c r="E95" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3778,11 +3496,8 @@
       <c r="D96" t="s">
         <v>511</v>
       </c>
-      <c r="E96" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3795,11 +3510,8 @@
       <c r="D97" t="s">
         <v>463</v>
       </c>
-      <c r="E97" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3812,11 +3524,8 @@
       <c r="D98" t="s">
         <v>512</v>
       </c>
-      <c r="E98" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3829,11 +3538,8 @@
       <c r="D99" t="s">
         <v>513</v>
       </c>
-      <c r="E99" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3846,11 +3552,8 @@
       <c r="D100" t="s">
         <v>463</v>
       </c>
-      <c r="E100" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3863,11 +3566,8 @@
       <c r="D101" t="s">
         <v>514</v>
       </c>
-      <c r="E101" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3880,11 +3580,8 @@
       <c r="D102" t="s">
         <v>463</v>
       </c>
-      <c r="E102" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3897,11 +3594,8 @@
       <c r="D103" t="s">
         <v>463</v>
       </c>
-      <c r="E103" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3914,11 +3608,8 @@
       <c r="D104" t="s">
         <v>463</v>
       </c>
-      <c r="E104" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3931,11 +3622,8 @@
       <c r="D105" t="s">
         <v>515</v>
       </c>
-      <c r="E105" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3948,11 +3636,8 @@
       <c r="D106" t="s">
         <v>463</v>
       </c>
-      <c r="E106" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3965,11 +3650,8 @@
       <c r="D107" t="s">
         <v>463</v>
       </c>
-      <c r="E107" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3982,11 +3664,8 @@
       <c r="D108" t="s">
         <v>516</v>
       </c>
-      <c r="E108" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3999,11 +3678,8 @@
       <c r="D109" t="s">
         <v>517</v>
       </c>
-      <c r="E109" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4016,11 +3692,8 @@
       <c r="D110" t="s">
         <v>518</v>
       </c>
-      <c r="E110" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4033,11 +3706,8 @@
       <c r="D111" t="s">
         <v>463</v>
       </c>
-      <c r="E111" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4050,11 +3720,8 @@
       <c r="D112" t="s">
         <v>519</v>
       </c>
-      <c r="E112" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4067,11 +3734,8 @@
       <c r="D113" t="s">
         <v>520</v>
       </c>
-      <c r="E113" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4084,11 +3748,8 @@
       <c r="D114" t="s">
         <v>521</v>
       </c>
-      <c r="E114" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4101,11 +3762,8 @@
       <c r="D115" t="s">
         <v>522</v>
       </c>
-      <c r="E115" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4118,11 +3776,8 @@
       <c r="D116" t="s">
         <v>463</v>
       </c>
-      <c r="E116" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4135,11 +3790,8 @@
       <c r="D117" t="s">
         <v>463</v>
       </c>
-      <c r="E117" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4152,11 +3804,8 @@
       <c r="D118" t="s">
         <v>523</v>
       </c>
-      <c r="E118" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4169,11 +3818,8 @@
       <c r="D119" t="s">
         <v>524</v>
       </c>
-      <c r="E119" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4186,11 +3832,8 @@
       <c r="D120" t="s">
         <v>525</v>
       </c>
-      <c r="E120" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4203,11 +3846,8 @@
       <c r="D121" t="s">
         <v>463</v>
       </c>
-      <c r="E121" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4220,11 +3860,8 @@
       <c r="D122" t="s">
         <v>526</v>
       </c>
-      <c r="E122" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4237,11 +3874,8 @@
       <c r="D123" t="s">
         <v>527</v>
       </c>
-      <c r="E123" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4254,11 +3888,8 @@
       <c r="D124" t="s">
         <v>463</v>
       </c>
-      <c r="E124" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4271,11 +3902,8 @@
       <c r="D125" t="s">
         <v>463</v>
       </c>
-      <c r="E125" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5">
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4288,11 +3916,8 @@
       <c r="D126" t="s">
         <v>463</v>
       </c>
-      <c r="E126" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4305,11 +3930,8 @@
       <c r="D127" t="s">
         <v>463</v>
       </c>
-      <c r="E127" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4322,11 +3944,8 @@
       <c r="D128" t="s">
         <v>528</v>
       </c>
-      <c r="E128" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4339,11 +3958,8 @@
       <c r="D129" t="s">
         <v>529</v>
       </c>
-      <c r="E129" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4356,11 +3972,8 @@
       <c r="D130" t="s">
         <v>530</v>
       </c>
-      <c r="E130" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4373,11 +3986,8 @@
       <c r="D131" t="s">
         <v>531</v>
       </c>
-      <c r="E131" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4390,11 +4000,8 @@
       <c r="D132" t="s">
         <v>463</v>
       </c>
-      <c r="E132" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4407,11 +4014,8 @@
       <c r="D133" t="s">
         <v>532</v>
       </c>
-      <c r="E133" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4424,11 +4028,8 @@
       <c r="D134" t="s">
         <v>463</v>
       </c>
-      <c r="E134" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4441,11 +4042,8 @@
       <c r="D135" t="s">
         <v>533</v>
       </c>
-      <c r="E135" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4458,11 +4056,8 @@
       <c r="D136" t="s">
         <v>534</v>
       </c>
-      <c r="E136" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4475,11 +4070,8 @@
       <c r="D137" t="s">
         <v>535</v>
       </c>
-      <c r="E137" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4492,11 +4084,8 @@
       <c r="D138" t="s">
         <v>536</v>
       </c>
-      <c r="E138" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4509,11 +4098,8 @@
       <c r="D139" t="s">
         <v>537</v>
       </c>
-      <c r="E139" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4526,11 +4112,8 @@
       <c r="D140" t="s">
         <v>538</v>
       </c>
-      <c r="E140" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4543,11 +4126,8 @@
       <c r="D141" t="s">
         <v>539</v>
       </c>
-      <c r="E141" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4560,11 +4140,8 @@
       <c r="D142" t="s">
         <v>540</v>
       </c>
-      <c r="E142" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4577,11 +4154,8 @@
       <c r="D143" t="s">
         <v>541</v>
       </c>
-      <c r="E143" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4594,11 +4168,8 @@
       <c r="D144" t="s">
         <v>463</v>
       </c>
-      <c r="E144" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4611,11 +4182,8 @@
       <c r="D145" t="s">
         <v>542</v>
       </c>
-      <c r="E145" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4628,11 +4196,8 @@
       <c r="D146" t="s">
         <v>543</v>
       </c>
-      <c r="E146" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4645,11 +4210,8 @@
       <c r="D147" t="s">
         <v>463</v>
       </c>
-      <c r="E147" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4662,11 +4224,8 @@
       <c r="D148" t="s">
         <v>544</v>
       </c>
-      <c r="E148" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4679,11 +4238,8 @@
       <c r="D149" t="s">
         <v>545</v>
       </c>
-      <c r="E149" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4696,11 +4252,8 @@
       <c r="D150" t="s">
         <v>546</v>
       </c>
-      <c r="E150" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4713,11 +4266,8 @@
       <c r="D151" t="s">
         <v>547</v>
       </c>
-      <c r="E151" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4730,11 +4280,8 @@
       <c r="D152" t="s">
         <v>548</v>
       </c>
-      <c r="E152" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4747,11 +4294,8 @@
       <c r="D153" t="s">
         <v>549</v>
       </c>
-      <c r="E153" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4764,11 +4308,8 @@
       <c r="D154" t="s">
         <v>550</v>
       </c>
-      <c r="E154" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4781,11 +4322,8 @@
       <c r="D155" t="s">
         <v>551</v>
       </c>
-      <c r="E155" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4798,11 +4336,8 @@
       <c r="D156" t="s">
         <v>463</v>
       </c>
-      <c r="E156" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4815,11 +4350,8 @@
       <c r="D157" t="s">
         <v>463</v>
       </c>
-      <c r="E157" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4832,11 +4364,8 @@
       <c r="D158" t="s">
         <v>552</v>
       </c>
-      <c r="E158" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4849,11 +4378,8 @@
       <c r="D159" t="s">
         <v>463</v>
       </c>
-      <c r="E159" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5">
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4866,11 +4392,8 @@
       <c r="D160" t="s">
         <v>463</v>
       </c>
-      <c r="E160" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4883,11 +4406,8 @@
       <c r="D161" t="s">
         <v>463</v>
       </c>
-      <c r="E161" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5">
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4900,11 +4420,8 @@
       <c r="D162" t="s">
         <v>553</v>
       </c>
-      <c r="E162" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5">
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4917,11 +4434,8 @@
       <c r="D163" t="s">
         <v>554</v>
       </c>
-      <c r="E163" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4934,11 +4448,8 @@
       <c r="D164" t="s">
         <v>463</v>
       </c>
-      <c r="E164" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5">
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4951,11 +4462,8 @@
       <c r="D165" t="s">
         <v>463</v>
       </c>
-      <c r="E165" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5">
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4968,11 +4476,8 @@
       <c r="D166" t="s">
         <v>555</v>
       </c>
-      <c r="E166" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5">
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4985,11 +4490,8 @@
       <c r="D167" t="s">
         <v>556</v>
       </c>
-      <c r="E167" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5002,11 +4504,8 @@
       <c r="D168" t="s">
         <v>557</v>
       </c>
-      <c r="E168" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5">
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5019,11 +4518,8 @@
       <c r="D169" t="s">
         <v>463</v>
       </c>
-      <c r="E169" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5">
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5036,11 +4532,8 @@
       <c r="D170" t="s">
         <v>558</v>
       </c>
-      <c r="E170" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5">
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5053,11 +4546,8 @@
       <c r="D171" t="s">
         <v>559</v>
       </c>
-      <c r="E171" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5">
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5070,11 +4560,8 @@
       <c r="D172" t="s">
         <v>560</v>
       </c>
-      <c r="E172" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5">
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5087,11 +4574,8 @@
       <c r="D173" t="s">
         <v>561</v>
       </c>
-      <c r="E173" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5">
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5104,11 +4588,8 @@
       <c r="D174" t="s">
         <v>562</v>
       </c>
-      <c r="E174" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5">
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5121,11 +4602,8 @@
       <c r="D175" t="s">
         <v>563</v>
       </c>
-      <c r="E175" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5">
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5138,11 +4616,8 @@
       <c r="D176" t="s">
         <v>564</v>
       </c>
-      <c r="E176" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5155,11 +4630,8 @@
       <c r="D177" t="s">
         <v>463</v>
       </c>
-      <c r="E177" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5172,11 +4644,8 @@
       <c r="D178" t="s">
         <v>463</v>
       </c>
-      <c r="E178" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5">
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5189,11 +4658,8 @@
       <c r="D179" t="s">
         <v>565</v>
       </c>
-      <c r="E179" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5206,11 +4672,8 @@
       <c r="D180" t="s">
         <v>566</v>
       </c>
-      <c r="E180" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5223,11 +4686,8 @@
       <c r="D181" t="s">
         <v>567</v>
       </c>
-      <c r="E181" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5240,11 +4700,8 @@
       <c r="D182" t="s">
         <v>463</v>
       </c>
-      <c r="E182" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5257,11 +4714,8 @@
       <c r="D183" t="s">
         <v>463</v>
       </c>
-      <c r="E183" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5">
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5274,11 +4728,8 @@
       <c r="D184" t="s">
         <v>463</v>
       </c>
-      <c r="E184" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5291,11 +4742,8 @@
       <c r="D185" t="s">
         <v>463</v>
       </c>
-      <c r="E185" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5">
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5308,11 +4756,8 @@
       <c r="D186" t="s">
         <v>463</v>
       </c>
-      <c r="E186" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5">
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5325,11 +4770,8 @@
       <c r="D187" t="s">
         <v>463</v>
       </c>
-      <c r="E187" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5">
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5342,11 +4784,8 @@
       <c r="D188" t="s">
         <v>568</v>
       </c>
-      <c r="E188" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5">
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5359,11 +4798,8 @@
       <c r="D189" t="s">
         <v>569</v>
       </c>
-      <c r="E189" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5">
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5376,11 +4812,8 @@
       <c r="D190" t="s">
         <v>570</v>
       </c>
-      <c r="E190" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5">
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5393,11 +4826,8 @@
       <c r="D191" t="s">
         <v>571</v>
       </c>
-      <c r="E191" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5">
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192">
         <v>191</v>
       </c>
@@ -5410,11 +4840,8 @@
       <c r="D192" t="s">
         <v>572</v>
       </c>
-      <c r="E192" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5">
+    </row>
+    <row r="193" spans="1:4">
       <c r="A193">
         <v>192</v>
       </c>
@@ -5427,11 +4854,8 @@
       <c r="D193" t="s">
         <v>463</v>
       </c>
-      <c r="E193" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5">
+    </row>
+    <row r="194" spans="1:4">
       <c r="A194">
         <v>193</v>
       </c>
@@ -5444,11 +4868,8 @@
       <c r="D194" t="s">
         <v>426</v>
       </c>
-      <c r="E194" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5">
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195">
         <v>194</v>
       </c>
@@ -5461,11 +4882,8 @@
       <c r="D195" t="s">
         <v>573</v>
       </c>
-      <c r="E195" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5">
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196">
         <v>195</v>
       </c>
@@ -5478,11 +4896,8 @@
       <c r="D196" t="s">
         <v>574</v>
       </c>
-      <c r="E196" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5">
+    </row>
+    <row r="197" spans="1:4">
       <c r="A197">
         <v>196</v>
       </c>
@@ -5495,11 +4910,8 @@
       <c r="D197" t="s">
         <v>463</v>
       </c>
-      <c r="E197" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5">
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198">
         <v>197</v>
       </c>
@@ -5512,11 +4924,8 @@
       <c r="D198" t="s">
         <v>463</v>
       </c>
-      <c r="E198" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5">
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199">
         <v>198</v>
       </c>
@@ -5529,11 +4938,8 @@
       <c r="D199" t="s">
         <v>575</v>
       </c>
-      <c r="E199" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5">
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200">
         <v>199</v>
       </c>
@@ -5546,11 +4952,8 @@
       <c r="D200" t="s">
         <v>576</v>
       </c>
-      <c r="E200" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5">
+    </row>
+    <row r="201" spans="1:4">
       <c r="A201">
         <v>200</v>
       </c>
@@ -5563,11 +4966,8 @@
       <c r="D201" t="s">
         <v>577</v>
       </c>
-      <c r="E201" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5">
+    </row>
+    <row r="202" spans="1:4">
       <c r="A202">
         <v>201</v>
       </c>
@@ -5580,11 +4980,8 @@
       <c r="D202" t="s">
         <v>463</v>
       </c>
-      <c r="E202" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5">
+    </row>
+    <row r="203" spans="1:4">
       <c r="A203">
         <v>202</v>
       </c>
@@ -5597,11 +4994,8 @@
       <c r="D203" t="s">
         <v>578</v>
       </c>
-      <c r="E203" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5">
+    </row>
+    <row r="204" spans="1:4">
       <c r="A204">
         <v>203</v>
       </c>
@@ -5614,11 +5008,8 @@
       <c r="D204" t="s">
         <v>436</v>
       </c>
-      <c r="E204" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5">
+    </row>
+    <row r="205" spans="1:4">
       <c r="A205">
         <v>204</v>
       </c>
@@ -5631,11 +5022,8 @@
       <c r="D205" t="s">
         <v>463</v>
       </c>
-      <c r="E205" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5">
+    </row>
+    <row r="206" spans="1:4">
       <c r="A206">
         <v>205</v>
       </c>
@@ -5648,11 +5036,8 @@
       <c r="D206" t="s">
         <v>463</v>
       </c>
-      <c r="E206" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5">
+    </row>
+    <row r="207" spans="1:4">
       <c r="A207">
         <v>206</v>
       </c>
@@ -5665,11 +5050,8 @@
       <c r="D207" t="s">
         <v>463</v>
       </c>
-      <c r="E207" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5">
+    </row>
+    <row r="208" spans="1:4">
       <c r="A208">
         <v>207</v>
       </c>
@@ -5682,11 +5064,8 @@
       <c r="D208" t="s">
         <v>463</v>
       </c>
-      <c r="E208" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5">
+    </row>
+    <row r="209" spans="1:4">
       <c r="A209">
         <v>208</v>
       </c>
@@ -5699,11 +5078,8 @@
       <c r="D209" t="s">
         <v>579</v>
       </c>
-      <c r="E209" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5">
+    </row>
+    <row r="210" spans="1:4">
       <c r="A210">
         <v>209</v>
       </c>
@@ -5716,11 +5092,8 @@
       <c r="D210" t="s">
         <v>580</v>
       </c>
-      <c r="E210" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5">
+    </row>
+    <row r="211" spans="1:4">
       <c r="A211">
         <v>210</v>
       </c>
@@ -5733,11 +5106,8 @@
       <c r="D211" t="s">
         <v>463</v>
       </c>
-      <c r="E211" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5">
+    </row>
+    <row r="212" spans="1:4">
       <c r="A212">
         <v>211</v>
       </c>
@@ -5750,11 +5120,8 @@
       <c r="D212" t="s">
         <v>581</v>
       </c>
-      <c r="E212" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5">
+    </row>
+    <row r="213" spans="1:4">
       <c r="A213">
         <v>212</v>
       </c>
@@ -5767,11 +5134,8 @@
       <c r="D213" t="s">
         <v>463</v>
       </c>
-      <c r="E213" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5">
+    </row>
+    <row r="214" spans="1:4">
       <c r="A214">
         <v>213</v>
       </c>
@@ -5784,11 +5148,8 @@
       <c r="D214" t="s">
         <v>582</v>
       </c>
-      <c r="E214" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5">
+    </row>
+    <row r="215" spans="1:4">
       <c r="A215">
         <v>214</v>
       </c>
@@ -5801,11 +5162,8 @@
       <c r="D215" t="s">
         <v>463</v>
       </c>
-      <c r="E215" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5">
+    </row>
+    <row r="216" spans="1:4">
       <c r="A216">
         <v>215</v>
       </c>
@@ -5818,11 +5176,8 @@
       <c r="D216" t="s">
         <v>583</v>
       </c>
-      <c r="E216" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5">
+    </row>
+    <row r="217" spans="1:4">
       <c r="A217">
         <v>216</v>
       </c>
@@ -5835,11 +5190,8 @@
       <c r="D217" t="s">
         <v>584</v>
       </c>
-      <c r="E217" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5">
+    </row>
+    <row r="218" spans="1:4">
       <c r="A218">
         <v>217</v>
       </c>
@@ -5852,11 +5204,8 @@
       <c r="D218" t="s">
         <v>585</v>
       </c>
-      <c r="E218" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5">
+    </row>
+    <row r="219" spans="1:4">
       <c r="A219">
         <v>218</v>
       </c>
@@ -5869,11 +5218,8 @@
       <c r="D219" t="s">
         <v>586</v>
       </c>
-      <c r="E219" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5">
+    </row>
+    <row r="220" spans="1:4">
       <c r="A220">
         <v>219</v>
       </c>
@@ -5886,11 +5232,8 @@
       <c r="D220" t="s">
         <v>463</v>
       </c>
-      <c r="E220" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5">
+    </row>
+    <row r="221" spans="1:4">
       <c r="A221">
         <v>220</v>
       </c>
@@ -5903,11 +5246,8 @@
       <c r="D221" t="s">
         <v>587</v>
       </c>
-      <c r="E221" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5">
+    </row>
+    <row r="222" spans="1:4">
       <c r="A222">
         <v>221</v>
       </c>
@@ -5920,11 +5260,8 @@
       <c r="D222" t="s">
         <v>463</v>
       </c>
-      <c r="E222" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5">
+    </row>
+    <row r="223" spans="1:4">
       <c r="A223">
         <v>222</v>
       </c>
@@ -5937,11 +5274,8 @@
       <c r="D223" t="s">
         <v>588</v>
       </c>
-      <c r="E223" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5">
+    </row>
+    <row r="224" spans="1:4">
       <c r="A224">
         <v>223</v>
       </c>
@@ -5954,11 +5288,8 @@
       <c r="D224" t="s">
         <v>589</v>
       </c>
-      <c r="E224" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5">
+    </row>
+    <row r="225" spans="1:4">
       <c r="A225">
         <v>224</v>
       </c>
@@ -5971,11 +5302,8 @@
       <c r="D225" t="s">
         <v>463</v>
       </c>
-      <c r="E225" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5">
+    </row>
+    <row r="226" spans="1:4">
       <c r="A226">
         <v>225</v>
       </c>
@@ -5988,11 +5316,8 @@
       <c r="D226" t="s">
         <v>463</v>
       </c>
-      <c r="E226" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5">
+    </row>
+    <row r="227" spans="1:4">
       <c r="A227">
         <v>226</v>
       </c>
@@ -6005,11 +5330,8 @@
       <c r="D227" t="s">
         <v>463</v>
       </c>
-      <c r="E227" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5">
+    </row>
+    <row r="228" spans="1:4">
       <c r="A228">
         <v>227</v>
       </c>
@@ -6022,11 +5344,8 @@
       <c r="D228" t="s">
         <v>590</v>
       </c>
-      <c r="E228" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5">
+    </row>
+    <row r="229" spans="1:4">
       <c r="A229">
         <v>228</v>
       </c>
@@ -6039,11 +5358,8 @@
       <c r="D229" t="s">
         <v>461</v>
       </c>
-      <c r="E229" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5">
+    </row>
+    <row r="230" spans="1:4">
       <c r="A230">
         <v>229</v>
       </c>
@@ -6054,9 +5370,6 @@
         <v>462</v>
       </c>
       <c r="D230" t="s">
-        <v>463</v>
-      </c>
-      <c r="E230" t="s">
         <v>463</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix combine merges for empty override check
</commit_message>
<xml_diff>
--- a/data/merge_bornpowerindex.xlsx
+++ b/data/merge_bornpowerindex.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="591">
   <si>
     <t>Index</t>
   </si>
@@ -2180,6 +2180,9 @@
       <c r="D2" t="s">
         <v>463</v>
       </c>
+      <c r="E2" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -2194,6 +2197,9 @@
       <c r="D3" t="s">
         <v>463</v>
       </c>
+      <c r="E3" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -2208,6 +2214,9 @@
       <c r="D4" t="s">
         <v>463</v>
       </c>
+      <c r="E4" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -2222,6 +2231,9 @@
       <c r="D5" t="s">
         <v>464</v>
       </c>
+      <c r="E5" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -2236,6 +2248,9 @@
       <c r="D6" t="s">
         <v>463</v>
       </c>
+      <c r="E6" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -2250,6 +2265,9 @@
       <c r="D7" t="s">
         <v>465</v>
       </c>
+      <c r="E7" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -2264,6 +2282,9 @@
       <c r="D8" t="s">
         <v>463</v>
       </c>
+      <c r="E8" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -2278,6 +2299,9 @@
       <c r="D9" t="s">
         <v>466</v>
       </c>
+      <c r="E9" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -2292,6 +2316,9 @@
       <c r="D10" t="s">
         <v>467</v>
       </c>
+      <c r="E10" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -2306,6 +2333,9 @@
       <c r="D11" t="s">
         <v>463</v>
       </c>
+      <c r="E11" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -2320,6 +2350,9 @@
       <c r="D12" t="s">
         <v>463</v>
       </c>
+      <c r="E12" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -2334,6 +2367,9 @@
       <c r="D13" t="s">
         <v>463</v>
       </c>
+      <c r="E13" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -2348,6 +2384,9 @@
       <c r="D14" t="s">
         <v>468</v>
       </c>
+      <c r="E14" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
@@ -2362,6 +2401,9 @@
       <c r="D15" t="s">
         <v>463</v>
       </c>
+      <c r="E15" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -2376,8 +2418,11 @@
       <c r="D16" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2390,8 +2435,11 @@
       <c r="D17" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2404,8 +2452,11 @@
       <c r="D18" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2418,8 +2469,11 @@
       <c r="D19" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2432,8 +2486,11 @@
       <c r="D20" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2446,8 +2503,11 @@
       <c r="D21" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2460,8 +2520,11 @@
       <c r="D22" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2474,8 +2537,11 @@
       <c r="D23" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2488,8 +2554,11 @@
       <c r="D24" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2502,8 +2571,11 @@
       <c r="D25" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2516,8 +2588,11 @@
       <c r="D26" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2530,8 +2605,11 @@
       <c r="D27" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2544,8 +2622,11 @@
       <c r="D28" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2558,8 +2639,11 @@
       <c r="D29" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2572,8 +2656,11 @@
       <c r="D30" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2586,8 +2673,11 @@
       <c r="D31" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2600,8 +2690,11 @@
       <c r="D32" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2614,8 +2707,11 @@
       <c r="D33" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2628,8 +2724,11 @@
       <c r="D34" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2642,8 +2741,11 @@
       <c r="D35" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2656,8 +2758,11 @@
       <c r="D36" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2670,8 +2775,11 @@
       <c r="D37" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2684,8 +2792,11 @@
       <c r="D38" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2698,8 +2809,11 @@
       <c r="D39" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2712,8 +2826,11 @@
       <c r="D40" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2726,8 +2843,11 @@
       <c r="D41" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2740,8 +2860,11 @@
       <c r="D42" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2754,8 +2877,11 @@
       <c r="D43" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2768,8 +2894,11 @@
       <c r="D44" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2782,8 +2911,11 @@
       <c r="D45" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2796,8 +2928,11 @@
       <c r="D46" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2810,8 +2945,11 @@
       <c r="D47" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2824,8 +2962,11 @@
       <c r="D48" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2838,8 +2979,11 @@
       <c r="D49" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2852,8 +2996,11 @@
       <c r="D50" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2866,8 +3013,11 @@
       <c r="D51" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2880,8 +3030,11 @@
       <c r="D52" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2894,8 +3047,11 @@
       <c r="D53" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2908,8 +3064,11 @@
       <c r="D54" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2922,8 +3081,11 @@
       <c r="D55" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2936,8 +3098,11 @@
       <c r="D56" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2950,8 +3115,11 @@
       <c r="D57" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2964,8 +3132,11 @@
       <c r="D58" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2978,8 +3149,11 @@
       <c r="D59" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2992,8 +3166,11 @@
       <c r="D60" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3006,8 +3183,11 @@
       <c r="D61" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3020,8 +3200,11 @@
       <c r="D62" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3034,8 +3217,11 @@
       <c r="D63" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3048,8 +3234,11 @@
       <c r="D64" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3062,8 +3251,11 @@
       <c r="D65" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3076,8 +3268,11 @@
       <c r="D66" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3090,8 +3285,11 @@
       <c r="D67" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3104,8 +3302,11 @@
       <c r="D68" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3118,8 +3319,11 @@
       <c r="D69" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3132,8 +3336,11 @@
       <c r="D70" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3146,8 +3353,11 @@
       <c r="D71" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3160,8 +3370,11 @@
       <c r="D72" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3174,8 +3387,11 @@
       <c r="D73" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3188,8 +3404,11 @@
       <c r="D74" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3202,8 +3421,11 @@
       <c r="D75" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3216,8 +3438,11 @@
       <c r="D76" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3230,8 +3455,11 @@
       <c r="D77" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3244,8 +3472,11 @@
       <c r="D78" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3258,8 +3489,11 @@
       <c r="D79" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3272,8 +3506,11 @@
       <c r="D80" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3286,8 +3523,11 @@
       <c r="D81" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3300,8 +3540,11 @@
       <c r="D82" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3314,8 +3557,11 @@
       <c r="D83" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3328,8 +3574,11 @@
       <c r="D84" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3342,8 +3591,11 @@
       <c r="D85" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3356,8 +3608,11 @@
       <c r="D86" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3370,8 +3625,11 @@
       <c r="D87" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3384,8 +3642,11 @@
       <c r="D88" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3398,8 +3659,11 @@
       <c r="D89" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3412,8 +3676,11 @@
       <c r="D90" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3426,8 +3693,11 @@
       <c r="D91" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3440,8 +3710,11 @@
       <c r="D92" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3454,8 +3727,11 @@
       <c r="D93" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3468,8 +3744,11 @@
       <c r="D94" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3482,8 +3761,11 @@
       <c r="D95" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3496,8 +3778,11 @@
       <c r="D96" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3510,8 +3795,11 @@
       <c r="D97" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3524,8 +3812,11 @@
       <c r="D98" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3538,8 +3829,11 @@
       <c r="D99" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3552,8 +3846,11 @@
       <c r="D100" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3566,8 +3863,11 @@
       <c r="D101" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3580,8 +3880,11 @@
       <c r="D102" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3594,8 +3897,11 @@
       <c r="D103" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3608,8 +3914,11 @@
       <c r="D104" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3622,8 +3931,11 @@
       <c r="D105" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3636,8 +3948,11 @@
       <c r="D106" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3650,8 +3965,11 @@
       <c r="D107" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3664,8 +3982,11 @@
       <c r="D108" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3678,8 +3999,11 @@
       <c r="D109" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3692,8 +4016,11 @@
       <c r="D110" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3706,8 +4033,11 @@
       <c r="D111" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3720,8 +4050,11 @@
       <c r="D112" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3734,8 +4067,11 @@
       <c r="D113" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3748,8 +4084,11 @@
       <c r="D114" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3762,8 +4101,11 @@
       <c r="D115" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3776,8 +4118,11 @@
       <c r="D116" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3790,8 +4135,11 @@
       <c r="D117" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3804,8 +4152,11 @@
       <c r="D118" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3818,8 +4169,11 @@
       <c r="D119" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3832,8 +4186,11 @@
       <c r="D120" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3846,8 +4203,11 @@
       <c r="D121" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3860,8 +4220,11 @@
       <c r="D122" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3874,8 +4237,11 @@
       <c r="D123" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3888,8 +4254,11 @@
       <c r="D124" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3902,8 +4271,11 @@
       <c r="D125" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3916,8 +4288,11 @@
       <c r="D126" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3930,8 +4305,11 @@
       <c r="D127" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3944,8 +4322,11 @@
       <c r="D128" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3958,8 +4339,11 @@
       <c r="D129" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3972,8 +4356,11 @@
       <c r="D130" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3986,8 +4373,11 @@
       <c r="D131" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4000,8 +4390,11 @@
       <c r="D132" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4014,8 +4407,11 @@
       <c r="D133" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4028,8 +4424,11 @@
       <c r="D134" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4042,8 +4441,11 @@
       <c r="D135" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4056,8 +4458,11 @@
       <c r="D136" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4070,8 +4475,11 @@
       <c r="D137" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4084,8 +4492,11 @@
       <c r="D138" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4098,8 +4509,11 @@
       <c r="D139" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4112,8 +4526,11 @@
       <c r="D140" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4126,8 +4543,11 @@
       <c r="D141" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4140,8 +4560,11 @@
       <c r="D142" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4154,8 +4577,11 @@
       <c r="D143" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4168,8 +4594,11 @@
       <c r="D144" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4182,8 +4611,11 @@
       <c r="D145" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4196,8 +4628,11 @@
       <c r="D146" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4210,8 +4645,11 @@
       <c r="D147" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4224,8 +4662,11 @@
       <c r="D148" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="E148" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4238,8 +4679,11 @@
       <c r="D149" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="E149" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4252,8 +4696,11 @@
       <c r="D150" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="E150" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4266,8 +4713,11 @@
       <c r="D151" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="E151" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4280,8 +4730,11 @@
       <c r="D152" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="E152" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4294,8 +4747,11 @@
       <c r="D153" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="E153" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4308,8 +4764,11 @@
       <c r="D154" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="E154" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4322,8 +4781,11 @@
       <c r="D155" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="E155" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4336,8 +4798,11 @@
       <c r="D156" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="E156" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4350,8 +4815,11 @@
       <c r="D157" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="E157" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4364,8 +4832,11 @@
       <c r="D158" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="E158" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4378,8 +4849,11 @@
       <c r="D159" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="E159" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4392,8 +4866,11 @@
       <c r="D160" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4406,8 +4883,11 @@
       <c r="D161" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4420,8 +4900,11 @@
       <c r="D162" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4434,8 +4917,11 @@
       <c r="D163" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="E163" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4448,8 +4934,11 @@
       <c r="D164" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="E164" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4462,8 +4951,11 @@
       <c r="D165" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="E165" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4476,8 +4968,11 @@
       <c r="D166" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="E166" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4490,8 +4985,11 @@
       <c r="D167" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="E167" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4504,8 +5002,11 @@
       <c r="D168" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="E168" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4518,8 +5019,11 @@
       <c r="D169" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="E169" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>169</v>
       </c>
@@ -4532,8 +5036,11 @@
       <c r="D170" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="E170" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>170</v>
       </c>
@@ -4546,8 +5053,11 @@
       <c r="D171" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="E171" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>171</v>
       </c>
@@ -4560,8 +5070,11 @@
       <c r="D172" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="E172" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>172</v>
       </c>
@@ -4574,8 +5087,11 @@
       <c r="D173" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="E173" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>173</v>
       </c>
@@ -4588,8 +5104,11 @@
       <c r="D174" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="E174" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>174</v>
       </c>
@@ -4602,8 +5121,11 @@
       <c r="D175" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="E175" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>175</v>
       </c>
@@ -4616,8 +5138,11 @@
       <c r="D176" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="177" spans="1:4">
+      <c r="E176" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>176</v>
       </c>
@@ -4630,8 +5155,11 @@
       <c r="D177" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="E177" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>177</v>
       </c>
@@ -4644,8 +5172,11 @@
       <c r="D178" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="E178" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>178</v>
       </c>
@@ -4658,8 +5189,11 @@
       <c r="D179" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="E179" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4672,8 +5206,11 @@
       <c r="D180" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="E180" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4686,8 +5223,11 @@
       <c r="D181" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="E181" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4700,8 +5240,11 @@
       <c r="D182" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="E182" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4714,8 +5257,11 @@
       <c r="D183" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="E183" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4728,8 +5274,11 @@
       <c r="D184" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="E184" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>184</v>
       </c>
@@ -4742,8 +5291,11 @@
       <c r="D185" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="186" spans="1:4">
+      <c r="E185" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4756,8 +5308,11 @@
       <c r="D186" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="E186" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>186</v>
       </c>
@@ -4770,8 +5325,11 @@
       <c r="D187" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="E187" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>187</v>
       </c>
@@ -4784,8 +5342,11 @@
       <c r="D188" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="E188" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>188</v>
       </c>
@@ -4798,8 +5359,11 @@
       <c r="D189" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="190" spans="1:4">
+      <c r="E189" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>189</v>
       </c>
@@ -4812,8 +5376,11 @@
       <c r="D190" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="E190" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>190</v>
       </c>
@@ -4826,8 +5393,11 @@
       <c r="D191" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="192" spans="1:4">
+      <c r="E191" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>191</v>
       </c>
@@ -4840,8 +5410,11 @@
       <c r="D192" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="E192" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>192</v>
       </c>
@@ -4854,8 +5427,11 @@
       <c r="D193" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="E193" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>193</v>
       </c>
@@ -4868,8 +5444,11 @@
       <c r="D194" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="195" spans="1:4">
+      <c r="E194" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>194</v>
       </c>
@@ -4882,8 +5461,11 @@
       <c r="D195" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="E195" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>195</v>
       </c>
@@ -4896,8 +5478,11 @@
       <c r="D196" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="E196" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>196</v>
       </c>
@@ -4910,8 +5495,11 @@
       <c r="D197" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="E197" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>197</v>
       </c>
@@ -4924,8 +5512,11 @@
       <c r="D198" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="E198" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>198</v>
       </c>
@@ -4938,8 +5529,11 @@
       <c r="D199" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="E199" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>199</v>
       </c>
@@ -4952,8 +5546,11 @@
       <c r="D200" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="E200" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
       <c r="A201">
         <v>200</v>
       </c>
@@ -4966,8 +5563,11 @@
       <c r="D201" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="202" spans="1:4">
+      <c r="E201" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
       <c r="A202">
         <v>201</v>
       </c>
@@ -4980,8 +5580,11 @@
       <c r="D202" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="203" spans="1:4">
+      <c r="E202" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
       <c r="A203">
         <v>202</v>
       </c>
@@ -4994,8 +5597,11 @@
       <c r="D203" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="E203" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
       <c r="A204">
         <v>203</v>
       </c>
@@ -5008,8 +5614,11 @@
       <c r="D204" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="E204" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
       <c r="A205">
         <v>204</v>
       </c>
@@ -5022,8 +5631,11 @@
       <c r="D205" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="E205" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
       <c r="A206">
         <v>205</v>
       </c>
@@ -5036,8 +5648,11 @@
       <c r="D206" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="E206" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
       <c r="A207">
         <v>206</v>
       </c>
@@ -5050,8 +5665,11 @@
       <c r="D207" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="E207" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
       <c r="A208">
         <v>207</v>
       </c>
@@ -5064,8 +5682,11 @@
       <c r="D208" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="209" spans="1:4">
+      <c r="E208" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
       <c r="A209">
         <v>208</v>
       </c>
@@ -5078,8 +5699,11 @@
       <c r="D209" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="210" spans="1:4">
+      <c r="E209" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
       <c r="A210">
         <v>209</v>
       </c>
@@ -5092,8 +5716,11 @@
       <c r="D210" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="211" spans="1:4">
+      <c r="E210" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
       <c r="A211">
         <v>210</v>
       </c>
@@ -5106,8 +5733,11 @@
       <c r="D211" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="212" spans="1:4">
+      <c r="E211" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212">
         <v>211</v>
       </c>
@@ -5120,8 +5750,11 @@
       <c r="D212" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="213" spans="1:4">
+      <c r="E212" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
       <c r="A213">
         <v>212</v>
       </c>
@@ -5134,8 +5767,11 @@
       <c r="D213" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="214" spans="1:4">
+      <c r="E213" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
       <c r="A214">
         <v>213</v>
       </c>
@@ -5148,8 +5784,11 @@
       <c r="D214" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="215" spans="1:4">
+      <c r="E214" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
       <c r="A215">
         <v>214</v>
       </c>
@@ -5162,8 +5801,11 @@
       <c r="D215" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="E215" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
       <c r="A216">
         <v>215</v>
       </c>
@@ -5176,8 +5818,11 @@
       <c r="D216" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="217" spans="1:4">
+      <c r="E216" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
       <c r="A217">
         <v>216</v>
       </c>
@@ -5190,8 +5835,11 @@
       <c r="D217" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="218" spans="1:4">
+      <c r="E217" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
       <c r="A218">
         <v>217</v>
       </c>
@@ -5204,8 +5852,11 @@
       <c r="D218" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="219" spans="1:4">
+      <c r="E218" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
       <c r="A219">
         <v>218</v>
       </c>
@@ -5218,8 +5869,11 @@
       <c r="D219" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="220" spans="1:4">
+      <c r="E219" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
       <c r="A220">
         <v>219</v>
       </c>
@@ -5232,8 +5886,11 @@
       <c r="D220" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="221" spans="1:4">
+      <c r="E220" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
       <c r="A221">
         <v>220</v>
       </c>
@@ -5246,8 +5903,11 @@
       <c r="D221" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="222" spans="1:4">
+      <c r="E221" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
       <c r="A222">
         <v>221</v>
       </c>
@@ -5260,8 +5920,11 @@
       <c r="D222" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="223" spans="1:4">
+      <c r="E222" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
       <c r="A223">
         <v>222</v>
       </c>
@@ -5274,8 +5937,11 @@
       <c r="D223" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="224" spans="1:4">
+      <c r="E223" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224">
         <v>223</v>
       </c>
@@ -5288,8 +5954,11 @@
       <c r="D224" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="225" spans="1:4">
+      <c r="E224" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
       <c r="A225">
         <v>224</v>
       </c>
@@ -5302,8 +5971,11 @@
       <c r="D225" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="226" spans="1:4">
+      <c r="E225" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
       <c r="A226">
         <v>225</v>
       </c>
@@ -5316,8 +5988,11 @@
       <c r="D226" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="227" spans="1:4">
+      <c r="E226" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
       <c r="A227">
         <v>226</v>
       </c>
@@ -5330,8 +6005,11 @@
       <c r="D227" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="228" spans="1:4">
+      <c r="E227" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
       <c r="A228">
         <v>227</v>
       </c>
@@ -5344,8 +6022,11 @@
       <c r="D228" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="229" spans="1:4">
+      <c r="E228" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
       <c r="A229">
         <v>228</v>
       </c>
@@ -5358,8 +6039,11 @@
       <c r="D229" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="230" spans="1:4">
+      <c r="E229" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
       <c r="A230">
         <v>229</v>
       </c>
@@ -5370,6 +6054,9 @@
         <v>462</v>
       </c>
       <c r="D230" t="s">
+        <v>463</v>
+      </c>
+      <c r="E230" t="s">
         <v>463</v>
       </c>
     </row>

</xml_diff>